<commit_message>
Curve fitting added and other fixes
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -495,7 +495,7 @@
         <v>0.125</v>
       </c>
       <c r="B5">
-        <v>-565.685424949238</v>
+        <v>-565.6854249492379</v>
       </c>
       <c r="C5">
         <v>-0.1</v>
@@ -633,7 +633,7 @@
         <v>0.375</v>
       </c>
       <c r="B11">
-        <v>565.685424949238</v>
+        <v>565.6854249492379</v>
       </c>
       <c r="C11">
         <v>1.100584418738097</v>
@@ -932,7 +932,7 @@
         <v>0.9166666666666666</v>
       </c>
       <c r="B24">
-        <v>-692.8203230275508</v>
+        <v>-692.8203230275507</v>
       </c>
       <c r="C24">
         <v>-0.1</v>
@@ -2427,10 +2427,10 @@
         <v>3.625</v>
       </c>
       <c r="B89">
-        <v>565.6854249492391</v>
+        <v>565.6854249492389</v>
       </c>
       <c r="C89">
-        <v>0.9906047811190727</v>
+        <v>0.9906047811190724</v>
       </c>
       <c r="D89">
         <v>0.2562314041861978</v>
@@ -3531,7 +3531,7 @@
         <v>5.625</v>
       </c>
       <c r="B137">
-        <v>565.6854249492392</v>
+        <v>565.6854249492393</v>
       </c>
       <c r="C137">
         <v>0.8450574884308553</v>
@@ -4359,7 +4359,7 @@
         <v>7.125</v>
       </c>
       <c r="B173">
-        <v>-565.6854249492415</v>
+        <v>-565.6854249492416</v>
       </c>
       <c r="C173">
         <v>-0.1</v>
@@ -5601,10 +5601,10 @@
         <v>9.375</v>
       </c>
       <c r="B227">
-        <v>565.6854249492392</v>
+        <v>565.6854249492393</v>
       </c>
       <c r="C227">
-        <v>0.5069603228231703</v>
+        <v>0.5069603228231705</v>
       </c>
       <c r="D227">
         <v>1.125475509344842</v>
@@ -5616,7 +5616,7 @@
         <v>0.00963505885337528</v>
       </c>
       <c r="G227">
-        <v>0.05474729781853528</v>
+        <v>0.05474729781853527</v>
       </c>
     </row>
     <row r="228" spans="1:7">
@@ -5639,7 +5639,7 @@
         <v>0.009627069678624587</v>
       </c>
       <c r="G228">
-        <v>0.05375664014944926</v>
+        <v>0.05375664014944925</v>
       </c>
     </row>
     <row r="229" spans="1:7">
@@ -5650,7 +5650,7 @@
         <v>772.7406610312541</v>
       </c>
       <c r="C229">
-        <v>0.6526741498334675</v>
+        <v>0.6526741498334676</v>
       </c>
       <c r="D229">
         <v>1.185215397836718</v>
@@ -5685,7 +5685,7 @@
         <v>0.00960917976250048</v>
       </c>
       <c r="G230">
-        <v>0.05153829055006</v>
+        <v>0.05153829055005999</v>
       </c>
     </row>
     <row r="231" spans="1:7">
@@ -5754,7 +5754,7 @@
         <v>0.009586810965782747</v>
       </c>
       <c r="G233">
-        <v>0.04876455975706114</v>
+        <v>0.04876455975706113</v>
       </c>
     </row>
     <row r="234" spans="1:7">
@@ -5777,7 +5777,7 @@
         <v>0.009582537600872387</v>
       </c>
       <c r="G234">
-        <v>0.04823466250817653</v>
+        <v>0.04823466250817652</v>
       </c>
     </row>
     <row r="235" spans="1:7">
@@ -5800,7 +5800,7 @@
         <v>0.009580347956844076</v>
       </c>
       <c r="G235">
-        <v>0.04796314664866595</v>
+        <v>0.04796314664866594</v>
       </c>
     </row>
     <row r="236" spans="1:7">
@@ -5823,7 +5823,7 @@
         <v>0.009580347956844076</v>
       </c>
       <c r="G236">
-        <v>0.04796314664866595</v>
+        <v>0.04796314664866593</v>
       </c>
     </row>
     <row r="237" spans="1:7">
@@ -5846,7 +5846,7 @@
         <v>0.009580347956844076</v>
       </c>
       <c r="G237">
-        <v>0.04796314664866595</v>
+        <v>0.04796314664866593</v>
       </c>
     </row>
     <row r="238" spans="1:7">
@@ -5869,7 +5869,7 @@
         <v>0.009580347956844076</v>
       </c>
       <c r="G238">
-        <v>0.04796314664866595</v>
+        <v>0.04796314664866593</v>
       </c>
     </row>
     <row r="239" spans="1:7">
@@ -5892,7 +5892,7 @@
         <v>0.009580347956844076</v>
       </c>
       <c r="G239">
-        <v>0.04796314664866595</v>
+        <v>0.04796314664866593</v>
       </c>
     </row>
     <row r="240" spans="1:7">
@@ -5915,7 +5915,7 @@
         <v>0.009580347956844076</v>
       </c>
       <c r="G240">
-        <v>0.04796314664866595</v>
+        <v>0.04796314664866593</v>
       </c>
     </row>
     <row r="241" spans="1:7">
@@ -5938,7 +5938,7 @@
         <v>0.009580347956844076</v>
       </c>
       <c r="G241">
-        <v>0.04796314664866595</v>
+        <v>0.04796314664866593</v>
       </c>
     </row>
     <row r="242" spans="1:7">
@@ -5961,7 +5961,7 @@
         <v>0.009580347956844076</v>
       </c>
       <c r="G242">
-        <v>0.04796314664866595</v>
+        <v>0.04796314664866593</v>
       </c>
     </row>
     <row r="243" spans="1:7">
@@ -5984,7 +5984,7 @@
         <v>0.009580347956844076</v>
       </c>
       <c r="G243">
-        <v>0.04796314664866595</v>
+        <v>0.04796314664866593</v>
       </c>
     </row>
     <row r="244" spans="1:7">
@@ -6007,7 +6007,7 @@
         <v>0.009580347956844076</v>
       </c>
       <c r="G244">
-        <v>0.04796314664866595</v>
+        <v>0.04796314664866593</v>
       </c>
     </row>
     <row r="245" spans="1:7">
@@ -6030,7 +6030,7 @@
         <v>0.009580347956844076</v>
       </c>
       <c r="G245">
-        <v>0.04796314664866595</v>
+        <v>0.04796314664866593</v>
       </c>
     </row>
     <row r="246" spans="1:7">
@@ -6053,7 +6053,7 @@
         <v>0.009580347956844076</v>
       </c>
       <c r="G246">
-        <v>0.04796314664866595</v>
+        <v>0.04796314664866593</v>
       </c>
     </row>
     <row r="247" spans="1:7">
@@ -6076,7 +6076,7 @@
         <v>0.009580347956844076</v>
       </c>
       <c r="G247">
-        <v>0.04796314664866595</v>
+        <v>0.04796314664866593</v>
       </c>
     </row>
     <row r="248" spans="1:7">
@@ -6099,7 +6099,7 @@
         <v>0.009580347956844076</v>
       </c>
       <c r="G248">
-        <v>0.04796314664866595</v>
+        <v>0.04796314664866593</v>
       </c>
     </row>
     <row r="249" spans="1:7">
@@ -6122,7 +6122,7 @@
         <v>0.00957808029202287</v>
       </c>
       <c r="G249">
-        <v>0.04768195621083649</v>
+        <v>0.04768195621083648</v>
       </c>
     </row>
     <row r="250" spans="1:7">
@@ -6133,7 +6133,7 @@
         <v>400.0000000000003</v>
       </c>
       <c r="C250">
-        <v>0.2941414242986025</v>
+        <v>0.2941414242986026</v>
       </c>
       <c r="D250">
         <v>1.278738118704672</v>
@@ -6145,7 +6145,7 @@
         <v>0.009573719073035706</v>
       </c>
       <c r="G250">
-        <v>0.04714116505642796</v>
+        <v>0.04714116505642794</v>
       </c>
     </row>
     <row r="251" spans="1:7">
@@ -6168,7 +6168,7 @@
         <v>0.009567607028169854</v>
       </c>
       <c r="G251">
-        <v>0.04638327149306239</v>
+        <v>0.04638327149306237</v>
       </c>
     </row>
     <row r="252" spans="1:7">
@@ -6191,7 +6191,7 @@
         <v>0.009560223399550899</v>
       </c>
       <c r="G252">
-        <v>0.04546770154431198</v>
+        <v>0.04546770154431197</v>
       </c>
     </row>
     <row r="253" spans="1:7">
@@ -6202,7 +6202,7 @@
         <v>772.7406610312541</v>
       </c>
       <c r="C253">
-        <v>0.5193297298373457</v>
+        <v>0.5193297298373456</v>
       </c>
       <c r="D253">
         <v>1.355354743849476</v>
@@ -6214,7 +6214,7 @@
         <v>0.009552136925107592</v>
       </c>
       <c r="G253">
-        <v>0.04446497871334187</v>
+        <v>0.04446497871334186</v>
       </c>
     </row>
     <row r="254" spans="1:7">
@@ -6225,7 +6225,7 @@
         <v>800</v>
       </c>
       <c r="C254">
-        <v>0.5147210473701196</v>
+        <v>0.5147210473701197</v>
       </c>
       <c r="D254">
         <v>1.384422644404153</v>
@@ -6237,7 +6237,7 @@
         <v>0.009543948784106275</v>
       </c>
       <c r="G254">
-        <v>0.04344964922917849</v>
+        <v>0.04344964922917847</v>
       </c>
     </row>
     <row r="255" spans="1:7">
@@ -6260,7 +6260,7 @@
         <v>0.009536234415990399</v>
       </c>
       <c r="G255">
-        <v>0.04249306758280993</v>
+        <v>0.04249306758280991</v>
       </c>
     </row>
     <row r="256" spans="1:7">
@@ -6268,7 +6268,7 @@
         <v>10.58333333333333</v>
       </c>
       <c r="B256">
-        <v>692.8203230275528</v>
+        <v>692.8203230275529</v>
       </c>
       <c r="C256">
         <v>0.4067128862442885</v>
@@ -6283,7 +6283,7 @@
         <v>0.009529494970317154</v>
       </c>
       <c r="G256">
-        <v>0.04165737631932748</v>
+        <v>0.04165737631932747</v>
       </c>
     </row>
     <row r="257" spans="1:7">
@@ -6306,7 +6306,7 @@
         <v>0.009524126673961063</v>
       </c>
       <c r="G257">
-        <v>0.04099170757117216</v>
+        <v>0.04099170757117215</v>
       </c>
     </row>
     <row r="258" spans="1:7">
@@ -6329,7 +6329,7 @@
         <v>0.009520410274344526</v>
       </c>
       <c r="G258">
-        <v>0.0405308740187215</v>
+        <v>0.04053087401872149</v>
       </c>
     </row>
     <row r="259" spans="1:7">
@@ -6352,7 +6352,7 @@
         <v>0.009518516066497392</v>
       </c>
       <c r="G259">
-        <v>0.04029599224567681</v>
+        <v>0.04029599224567679</v>
       </c>
     </row>
     <row r="260" spans="1:7">
@@ -6375,7 +6375,7 @@
         <v>0.009518516066497392</v>
       </c>
       <c r="G260">
-        <v>0.04029599224567681</v>
+        <v>0.04029599224567679</v>
       </c>
     </row>
     <row r="261" spans="1:7">
@@ -6398,7 +6398,7 @@
         <v>0.009518516066497392</v>
       </c>
       <c r="G261">
-        <v>0.04029599224567681</v>
+        <v>0.04029599224567679</v>
       </c>
     </row>
     <row r="262" spans="1:7">
@@ -6421,7 +6421,7 @@
         <v>0.009518516066497392</v>
       </c>
       <c r="G262">
-        <v>0.04029599224567681</v>
+        <v>0.04029599224567679</v>
       </c>
     </row>
     <row r="263" spans="1:7">
@@ -6444,7 +6444,7 @@
         <v>0.009518516066497392</v>
       </c>
       <c r="G263">
-        <v>0.04029599224567681</v>
+        <v>0.04029599224567679</v>
       </c>
     </row>
     <row r="264" spans="1:7">
@@ -6467,7 +6467,7 @@
         <v>0.009518516066497392</v>
       </c>
       <c r="G264">
-        <v>0.04029599224567681</v>
+        <v>0.04029599224567679</v>
       </c>
     </row>
     <row r="265" spans="1:7">
@@ -6490,7 +6490,7 @@
         <v>0.009518516066497392</v>
       </c>
       <c r="G265">
-        <v>0.04029599224567681</v>
+        <v>0.04029599224567679</v>
       </c>
     </row>
     <row r="266" spans="1:7">
@@ -6513,7 +6513,7 @@
         <v>0.009518516066497392</v>
       </c>
       <c r="G266">
-        <v>0.04029599224567681</v>
+        <v>0.04029599224567679</v>
       </c>
     </row>
     <row r="267" spans="1:7">
@@ -6536,7 +6536,7 @@
         <v>0.009518516066497392</v>
       </c>
       <c r="G267">
-        <v>0.04029599224567681</v>
+        <v>0.04029599224567679</v>
       </c>
     </row>
     <row r="268" spans="1:7">
@@ -6559,7 +6559,7 @@
         <v>0.009518516066497392</v>
       </c>
       <c r="G268">
-        <v>0.04029599224567681</v>
+        <v>0.04029599224567679</v>
       </c>
     </row>
     <row r="269" spans="1:7">
@@ -6582,7 +6582,7 @@
         <v>0.009518516066497392</v>
       </c>
       <c r="G269">
-        <v>0.04029599224567681</v>
+        <v>0.04029599224567679</v>
       </c>
     </row>
     <row r="270" spans="1:7">
@@ -6605,7 +6605,7 @@
         <v>0.009518516066497392</v>
       </c>
       <c r="G270">
-        <v>0.04029599224567681</v>
+        <v>0.04029599224567679</v>
       </c>
     </row>
     <row r="271" spans="1:7">
@@ -6628,7 +6628,7 @@
         <v>0.009518516066497392</v>
       </c>
       <c r="G271">
-        <v>0.04029599224567681</v>
+        <v>0.04029599224567679</v>
       </c>
     </row>
     <row r="272" spans="1:7">
@@ -6651,7 +6651,7 @@
         <v>0.009518516066497392</v>
       </c>
       <c r="G272">
-        <v>0.0402959922456768</v>
+        <v>0.04029599224567679</v>
       </c>
     </row>
     <row r="273" spans="1:7">
@@ -6674,7 +6674,7 @@
         <v>0.009516483884901445</v>
       </c>
       <c r="G273">
-        <v>0.04004400172777939</v>
+        <v>0.04004400172777938</v>
       </c>
     </row>
     <row r="274" spans="1:7">
@@ -6697,7 +6697,7 @@
         <v>0.009512585492127653</v>
       </c>
       <c r="G274">
-        <v>0.03956060102382918</v>
+        <v>0.03956060102382916</v>
       </c>
     </row>
     <row r="275" spans="1:7">
@@ -6705,10 +6705,10 @@
         <v>11.375</v>
       </c>
       <c r="B275">
-        <v>565.6854249492391</v>
+        <v>565.6854249492389</v>
       </c>
       <c r="C275">
-        <v>0.3253543508161417</v>
+        <v>0.3253543508161418</v>
       </c>
       <c r="D275">
         <v>1.442993613251588</v>
@@ -6720,7 +6720,7 @@
         <v>0.00950714881553597</v>
       </c>
       <c r="G275">
-        <v>0.03888645312646053</v>
+        <v>0.03888645312646052</v>
       </c>
     </row>
     <row r="276" spans="1:7">
@@ -6743,7 +6743,7 @@
         <v>0.009500626099028263</v>
       </c>
       <c r="G276">
-        <v>0.03807763627950485</v>
+        <v>0.03807763627950484</v>
       </c>
     </row>
     <row r="277" spans="1:7">
@@ -6751,10 +6751,10 @@
         <v>11.45833333333333</v>
       </c>
       <c r="B277">
-        <v>772.7406610312527</v>
+        <v>772.7406610312526</v>
       </c>
       <c r="C277">
-        <v>0.4116898046223035</v>
+        <v>0.4116898046223034</v>
       </c>
       <c r="D277">
         <v>1.49129920273317</v>
@@ -6766,7 +6766,7 @@
         <v>0.009493541607231299</v>
       </c>
       <c r="G277">
-        <v>0.03719915929668131</v>
+        <v>0.0371991592966813</v>
       </c>
     </row>
     <row r="278" spans="1:7">
@@ -6789,7 +6789,7 @@
         <v>0.009486432961897221</v>
       </c>
       <c r="G278">
-        <v>0.03631768727525558</v>
+        <v>0.03631768727525557</v>
       </c>
     </row>
     <row r="279" spans="1:7">
@@ -6812,7 +6812,7 @@
         <v>0.009479796855113408</v>
       </c>
       <c r="G279">
-        <v>0.03549481003406274</v>
+        <v>0.03549481003406273</v>
       </c>
     </row>
     <row r="280" spans="1:7">
@@ -6835,7 +6835,7 @@
         <v>0.009474049180347522</v>
       </c>
       <c r="G280">
-        <v>0.03478209836309281</v>
+        <v>0.0347820983630928</v>
       </c>
     </row>
     <row r="281" spans="1:7">
@@ -6858,7 +6858,7 @@
         <v>0.009469505084222072</v>
       </c>
       <c r="G281">
-        <v>0.03421863044353693</v>
+        <v>0.03421863044353692</v>
       </c>
     </row>
     <row r="282" spans="1:7">
@@ -6881,7 +6881,7 @@
         <v>0.009466377901850275</v>
       </c>
       <c r="G282">
-        <v>0.0338308598294341</v>
+        <v>0.03383085982943409</v>
       </c>
     </row>
     <row r="283" spans="1:7">
@@ -6904,7 +6904,7 @@
         <v>0.009464790514352799</v>
       </c>
       <c r="G283">
-        <v>0.033634023779747</v>
+        <v>0.03363402377974698</v>
       </c>
     </row>
     <row r="284" spans="1:7">
@@ -6927,7 +6927,7 @@
         <v>0.009464790514352799</v>
       </c>
       <c r="G284">
-        <v>0.03363402377974699</v>
+        <v>0.03363402377974697</v>
       </c>
     </row>
     <row r="285" spans="1:7">
@@ -6950,7 +6950,7 @@
         <v>0.009464790514352799</v>
       </c>
       <c r="G285">
-        <v>0.03363402377974699</v>
+        <v>0.03363402377974697</v>
       </c>
     </row>
     <row r="286" spans="1:7">
@@ -6958,7 +6958,7 @@
         <v>11.83333333333333</v>
       </c>
       <c r="B286">
-        <v>-399.9999999999976</v>
+        <v>-399.9999999999977</v>
       </c>
       <c r="C286">
         <v>-0.1</v>
@@ -6973,7 +6973,7 @@
         <v>0.009464790514352799</v>
       </c>
       <c r="G286">
-        <v>0.03363402377974699</v>
+        <v>0.03363402377974697</v>
       </c>
     </row>
     <row r="287" spans="1:7">
@@ -6996,7 +6996,7 @@
         <v>0.009464790514352799</v>
       </c>
       <c r="G287">
-        <v>0.03363402377974699</v>
+        <v>0.03363402377974697</v>
       </c>
     </row>
     <row r="288" spans="1:7">
@@ -7019,7 +7019,7 @@
         <v>0.009464790514352799</v>
       </c>
       <c r="G288">
-        <v>0.03363402377974699</v>
+        <v>0.03363402377974697</v>
       </c>
     </row>
     <row r="289" spans="1:7">
@@ -7042,7 +7042,7 @@
         <v>0.009464790514352799</v>
       </c>
       <c r="G289">
-        <v>0.03363402377974699</v>
+        <v>0.03363402377974697</v>
       </c>
     </row>
     <row r="290" spans="1:7">
@@ -7065,7 +7065,7 @@
         <v>0.009464790514352799</v>
       </c>
       <c r="G290">
-        <v>0.03363402377974699</v>
+        <v>0.03363402377974697</v>
       </c>
     </row>
     <row r="291" spans="1:7">
@@ -7088,7 +7088,7 @@
         <v>0.009464790514352799</v>
       </c>
       <c r="G291">
-        <v>0.03363402377974699</v>
+        <v>0.03363402377974697</v>
       </c>
     </row>
     <row r="292" spans="1:7">
@@ -7111,7 +7111,7 @@
         <v>0.009464790514352799</v>
       </c>
       <c r="G292">
-        <v>0.03363402377974699</v>
+        <v>0.03363402377974697</v>
       </c>
     </row>
     <row r="293" spans="1:7">
@@ -7134,7 +7134,7 @@
         <v>0.009464790514352799</v>
       </c>
       <c r="G293">
-        <v>0.03363402377974699</v>
+        <v>0.03363402377974697</v>
       </c>
     </row>
     <row r="294" spans="1:7">
@@ -7157,7 +7157,7 @@
         <v>0.009464790514352799</v>
       </c>
       <c r="G294">
-        <v>0.03363402377974699</v>
+        <v>0.03363402377974697</v>
       </c>
     </row>
     <row r="295" spans="1:7">
@@ -7180,7 +7180,7 @@
         <v>0.009464790514352799</v>
       </c>
       <c r="G295">
-        <v>0.03363402377974699</v>
+        <v>0.03363402377974697</v>
       </c>
     </row>
     <row r="296" spans="1:7">
@@ -7203,7 +7203,7 @@
         <v>0.009464790514352799</v>
       </c>
       <c r="G296">
-        <v>0.03363402377974699</v>
+        <v>0.03363402377974697</v>
       </c>
     </row>
     <row r="297" spans="1:7">
@@ -7226,7 +7226,7 @@
         <v>0.009463009883677194</v>
       </c>
       <c r="G297">
-        <v>0.03341322557597189</v>
+        <v>0.03341322557597188</v>
       </c>
     </row>
     <row r="298" spans="1:7">
@@ -7249,7 +7249,7 @@
         <v>0.009459600706354359</v>
       </c>
       <c r="G298">
-        <v>0.03299048758794043</v>
+        <v>0.03299048758794042</v>
       </c>
     </row>
     <row r="299" spans="1:7">
@@ -7272,7 +7272,7 @@
         <v>0.009454864103103535</v>
       </c>
       <c r="G299">
-        <v>0.03240314878483829</v>
+        <v>0.03240314878483828</v>
       </c>
     </row>
     <row r="300" spans="1:7">
@@ -7295,7 +7295,7 @@
         <v>0.009449211046922134</v>
       </c>
       <c r="G300">
-        <v>0.03170216981834462</v>
+        <v>0.0317021698183446</v>
       </c>
     </row>
     <row r="301" spans="1:7">
@@ -7318,7 +7318,7 @@
         <v>0.009443109688829478</v>
       </c>
       <c r="G301">
-        <v>0.03094560141485526</v>
+        <v>0.03094560141485525</v>
       </c>
     </row>
     <row r="302" spans="1:7">
@@ -7341,7 +7341,7 @@
         <v>0.009437029291761921</v>
       </c>
       <c r="G302">
-        <v>0.03019163217847835</v>
+        <v>0.03019163217847834</v>
       </c>
     </row>
     <row r="303" spans="1:7">
@@ -7364,7 +7364,7 @@
         <v>0.00943139188469885</v>
       </c>
       <c r="G303">
-        <v>0.02949259370265752</v>
+        <v>0.02949259370265751</v>
       </c>
     </row>
     <row r="304" spans="1:7">
@@ -7387,7 +7387,7 @@
         <v>0.009426540289270457</v>
       </c>
       <c r="G304">
-        <v>0.02889099586953683</v>
+        <v>0.02889099586953681</v>
       </c>
     </row>
     <row r="305" spans="1:7">
@@ -7410,7 +7410,7 @@
         <v>0.009422725703986392</v>
       </c>
       <c r="G305">
-        <v>0.02841798729431261</v>
+        <v>0.0284179872943126</v>
       </c>
     </row>
     <row r="306" spans="1:7">
@@ -7433,7 +7433,7 @@
         <v>0.009420111909500142</v>
       </c>
       <c r="G306">
-        <v>0.02809387677801777</v>
+        <v>0.02809387677801775</v>
       </c>
     </row>
     <row r="307" spans="1:7">
@@ -7456,7 +7456,7 @@
         <v>0.00941878904841691</v>
       </c>
       <c r="G307">
-        <v>0.02792984200369688</v>
+        <v>0.02792984200369687</v>
       </c>
     </row>
     <row r="308" spans="1:7">
@@ -7479,7 +7479,7 @@
         <v>0.00941878904841691</v>
       </c>
       <c r="G308">
-        <v>0.02792984200369688</v>
+        <v>0.02792984200369687</v>
       </c>
     </row>
     <row r="309" spans="1:7">
@@ -7502,7 +7502,7 @@
         <v>0.00941878904841691</v>
       </c>
       <c r="G309">
-        <v>0.02792984200369688</v>
+        <v>0.02792984200369687</v>
       </c>
     </row>
     <row r="310" spans="1:7">
@@ -7525,7 +7525,7 @@
         <v>0.00941878904841691</v>
       </c>
       <c r="G310">
-        <v>0.02792984200369688</v>
+        <v>0.02792984200369687</v>
       </c>
     </row>
     <row r="311" spans="1:7">
@@ -7548,7 +7548,7 @@
         <v>0.00941878904841691</v>
       </c>
       <c r="G311">
-        <v>0.02792984200369688</v>
+        <v>0.02792984200369687</v>
       </c>
     </row>
     <row r="312" spans="1:7">
@@ -7571,7 +7571,7 @@
         <v>0.00941878904841691</v>
       </c>
       <c r="G312">
-        <v>0.02792984200369688</v>
+        <v>0.02792984200369687</v>
       </c>
     </row>
     <row r="313" spans="1:7">
@@ -7594,7 +7594,7 @@
         <v>0.00941878904841691</v>
       </c>
       <c r="G313">
-        <v>0.02792984200369688</v>
+        <v>0.02792984200369687</v>
       </c>
     </row>
     <row r="314" spans="1:7">
@@ -7617,7 +7617,7 @@
         <v>0.00941878904841691</v>
       </c>
       <c r="G314">
-        <v>0.02792984200369688</v>
+        <v>0.02792984200369687</v>
       </c>
     </row>
     <row r="315" spans="1:7">
@@ -7640,7 +7640,7 @@
         <v>0.00941878904841691</v>
       </c>
       <c r="G315">
-        <v>0.02792984200369688</v>
+        <v>0.02792984200369687</v>
       </c>
     </row>
     <row r="316" spans="1:7">
@@ -7663,7 +7663,7 @@
         <v>0.00941878904841691</v>
       </c>
       <c r="G316">
-        <v>0.02792984200369688</v>
+        <v>0.02792984200369687</v>
       </c>
     </row>
     <row r="317" spans="1:7">
@@ -7686,7 +7686,7 @@
         <v>0.00941878904841691</v>
       </c>
       <c r="G317">
-        <v>0.02792984200369688</v>
+        <v>0.02792984200369687</v>
       </c>
     </row>
     <row r="318" spans="1:7">
@@ -7709,7 +7709,7 @@
         <v>0.00941878904841691</v>
       </c>
       <c r="G318">
-        <v>0.02792984200369688</v>
+        <v>0.02792984200369687</v>
       </c>
     </row>
     <row r="319" spans="1:7">
@@ -7732,7 +7732,7 @@
         <v>0.00941878904841691</v>
       </c>
       <c r="G319">
-        <v>0.02792984200369688</v>
+        <v>0.02792984200369687</v>
       </c>
     </row>
     <row r="320" spans="1:7">
@@ -7755,7 +7755,7 @@
         <v>0.00941878904841691</v>
       </c>
       <c r="G320">
-        <v>0.02792984200369688</v>
+        <v>0.02792984200369687</v>
       </c>
     </row>
     <row r="321" spans="1:7">
@@ -7766,7 +7766,7 @@
         <v>207.0552360820153</v>
       </c>
       <c r="C321">
-        <v>0.08467666247642244</v>
+        <v>0.08467666247642243</v>
       </c>
       <c r="D321">
         <v>1.595717161078608</v>
@@ -7778,7 +7778,7 @@
         <v>0.009417208708629166</v>
       </c>
       <c r="G321">
-        <v>0.02773387987001671</v>
+        <v>0.0277338798700167</v>
       </c>
     </row>
     <row r="322" spans="1:7">
@@ -7789,7 +7789,7 @@
         <v>399.9999999999949</v>
       </c>
       <c r="C322">
-        <v>0.1613427300729986</v>
+        <v>0.1613427300729985</v>
       </c>
       <c r="D322">
         <v>1.60644455121164</v>
@@ -7801,7 +7801,7 @@
         <v>0.009414186908591691</v>
       </c>
       <c r="G322">
-        <v>0.02735917666536997</v>
+        <v>0.02735917666536996</v>
       </c>
     </row>
     <row r="323" spans="1:7">
@@ -7824,7 +7824,7 @@
         <v>0.009409998919075364</v>
       </c>
       <c r="G323">
-        <v>0.02683986596534526</v>
+        <v>0.02683986596534525</v>
       </c>
     </row>
     <row r="324" spans="1:7">
@@ -7847,7 +7847,7 @@
         <v>0.00940501788194415</v>
       </c>
       <c r="G324">
-        <v>0.02622221736107466</v>
+        <v>0.02622221736107464</v>
       </c>
     </row>
     <row r="325" spans="1:7">
@@ -7870,7 +7870,7 @@
         <v>0.009399664033854791</v>
       </c>
       <c r="G325">
-        <v>0.02555834019799424</v>
+        <v>0.02555834019799422</v>
       </c>
     </row>
     <row r="326" spans="1:7">
@@ -7893,7 +7893,7 @@
         <v>0.00939435237997833</v>
       </c>
       <c r="G326">
-        <v>0.02489969511731309</v>
+        <v>0.02489969511731308</v>
       </c>
     </row>
     <row r="327" spans="1:7">
@@ -7916,7 +7916,7 @@
         <v>0.009389449596709232</v>
       </c>
       <c r="G327">
-        <v>0.0242917499919449</v>
+        <v>0.02429174999194489</v>
       </c>
     </row>
     <row r="328" spans="1:7">
@@ -7939,7 +7939,7 @@
         <v>0.009385247581504894</v>
       </c>
       <c r="G328">
-        <v>0.0237707001066071</v>
+        <v>0.02377070010660709</v>
       </c>
     </row>
     <row r="329" spans="1:7">
@@ -7962,7 +7962,7 @@
         <v>0.00938195539054526</v>
       </c>
       <c r="G329">
-        <v>0.0233624684276126</v>
+        <v>0.02336246842761258</v>
       </c>
     </row>
     <row r="330" spans="1:7">
@@ -7985,7 +7985,7 @@
         <v>0.009379705777044953</v>
       </c>
       <c r="G330">
-        <v>0.02308351635357456</v>
+        <v>0.02308351635357455</v>
       </c>
     </row>
     <row r="331" spans="1:7">
@@ -8008,7 +8008,7 @@
         <v>0.009378569373466518</v>
       </c>
       <c r="G331">
-        <v>0.02294260230984858</v>
+        <v>0.02294260230984857</v>
       </c>
     </row>
     <row r="332" spans="1:7">
@@ -8031,7 +8031,7 @@
         <v>0.009378569373466518</v>
       </c>
       <c r="G332">
-        <v>0.02294260230984858</v>
+        <v>0.02294260230984856</v>
       </c>
     </row>
     <row r="333" spans="1:7">
@@ -8054,7 +8054,7 @@
         <v>0.009378569373466518</v>
       </c>
       <c r="G333">
-        <v>0.02294260230984858</v>
+        <v>0.02294260230984856</v>
       </c>
     </row>
     <row r="334" spans="1:7">
@@ -8077,7 +8077,7 @@
         <v>0.009378569373466518</v>
       </c>
       <c r="G334">
-        <v>0.02294260230984858</v>
+        <v>0.02294260230984856</v>
       </c>
     </row>
     <row r="335" spans="1:7">
@@ -8100,7 +8100,7 @@
         <v>0.009378569373466518</v>
       </c>
       <c r="G335">
-        <v>0.02294260230984858</v>
+        <v>0.02294260230984856</v>
       </c>
     </row>
     <row r="336" spans="1:7">
@@ -8123,7 +8123,7 @@
         <v>0.009378569373466518</v>
       </c>
       <c r="G336">
-        <v>0.02294260230984858</v>
+        <v>0.02294260230984856</v>
       </c>
     </row>
     <row r="337" spans="1:7">
@@ -8146,7 +8146,7 @@
         <v>0.009378569373466518</v>
       </c>
       <c r="G337">
-        <v>0.02294260230984858</v>
+        <v>0.02294260230984856</v>
       </c>
     </row>
     <row r="338" spans="1:7">
@@ -8169,7 +8169,7 @@
         <v>0.009378569373466518</v>
       </c>
       <c r="G338">
-        <v>0.02294260230984858</v>
+        <v>0.02294260230984856</v>
       </c>
     </row>
     <row r="339" spans="1:7">
@@ -8192,7 +8192,7 @@
         <v>0.009378569373466518</v>
       </c>
       <c r="G339">
-        <v>0.02294260230984858</v>
+        <v>0.02294260230984856</v>
       </c>
     </row>
     <row r="340" spans="1:7">
@@ -8215,7 +8215,7 @@
         <v>0.009378569373466518</v>
       </c>
       <c r="G340">
-        <v>0.02294260230984858</v>
+        <v>0.02294260230984856</v>
       </c>
     </row>
     <row r="341" spans="1:7">
@@ -8238,7 +8238,7 @@
         <v>0.009378569373466518</v>
       </c>
       <c r="G341">
-        <v>0.02294260230984858</v>
+        <v>0.02294260230984856</v>
       </c>
     </row>
     <row r="342" spans="1:7">
@@ -8261,7 +8261,7 @@
         <v>0.009378569373466518</v>
       </c>
       <c r="G342">
-        <v>0.02294260230984858</v>
+        <v>0.02294260230984856</v>
       </c>
     </row>
     <row r="343" spans="1:7">
@@ -8284,7 +8284,7 @@
         <v>0.009378569373466518</v>
       </c>
       <c r="G343">
-        <v>0.02294260230984858</v>
+        <v>0.02294260230984856</v>
       </c>
     </row>
     <row r="344" spans="1:7">
@@ -8307,7 +8307,7 @@
         <v>0.009378569373466518</v>
       </c>
       <c r="G344">
-        <v>0.02294260230984858</v>
+        <v>0.02294260230984856</v>
       </c>
     </row>
     <row r="345" spans="1:7">
@@ -8330,7 +8330,7 @@
         <v>0.009377163742896129</v>
       </c>
       <c r="G345">
-        <v>0.02276830411912047</v>
+        <v>0.02276830411912045</v>
       </c>
     </row>
     <row r="346" spans="1:7">
@@ -8353,7 +8353,7 @@
         <v>0.009374478708353803</v>
       </c>
       <c r="G346">
-        <v>0.02243535983587193</v>
+        <v>0.02243535983587192</v>
       </c>
     </row>
     <row r="347" spans="1:7">
@@ -8376,7 +8376,7 @@
         <v>0.009370764630660808</v>
       </c>
       <c r="G347">
-        <v>0.02197481420194059</v>
+        <v>0.02197481420194057</v>
       </c>
     </row>
     <row r="348" spans="1:7">
@@ -8399,7 +8399,7 @@
         <v>0.00936635910123753</v>
       </c>
       <c r="G348">
-        <v>0.02142852855345413</v>
+        <v>0.02142852855345411</v>
       </c>
     </row>
     <row r="349" spans="1:7">
@@ -8422,7 +8422,7 @@
         <v>0.009361638990063545</v>
       </c>
       <c r="G349">
-        <v>0.02084323476788001</v>
+        <v>0.02084323476788</v>
       </c>
     </row>
     <row r="350" spans="1:7">
@@ -8445,7 +8445,7 @@
         <v>0.009356972211684933</v>
       </c>
       <c r="G350">
-        <v>0.02026455424893213</v>
+        <v>0.02026455424893212</v>
       </c>
     </row>
     <row r="351" spans="1:7">
@@ -8468,7 +8468,7 @@
         <v>0.009352679387937331</v>
       </c>
       <c r="G351">
-        <v>0.01973224410422937</v>
+        <v>0.01973224410422936</v>
       </c>
     </row>
     <row r="352" spans="1:7">
@@ -8491,7 +8491,7 @@
         <v>0.009349011739326937</v>
       </c>
       <c r="G352">
-        <v>0.01927745567654055</v>
+        <v>0.01927745567654053</v>
       </c>
     </row>
     <row r="353" spans="1:7">
@@ -8499,7 +8499,7 @@
         <v>14.625</v>
       </c>
       <c r="B353">
-        <v>565.6854249492366</v>
+        <v>565.6854249492364</v>
       </c>
       <c r="C353">
         <v>0.1392740347134357</v>
@@ -8514,7 +8514,7 @@
         <v>0.009346145946651938</v>
       </c>
       <c r="G353">
-        <v>0.01892209738484062</v>
+        <v>0.0189220973848406</v>
       </c>
     </row>
     <row r="354" spans="1:7">
@@ -8537,7 +8537,7 @@
         <v>0.009344191808204663</v>
       </c>
       <c r="G354">
-        <v>0.0186797842173785</v>
+        <v>0.01867978421737848</v>
       </c>
     </row>
     <row r="355" spans="1:7">
@@ -8560,7 +8560,7 @@
         <v>0.009343206072515067</v>
       </c>
       <c r="G355">
-        <v>0.01855755299186847</v>
+        <v>0.01855755299186845</v>
       </c>
     </row>
     <row r="356" spans="1:7">
@@ -8583,7 +8583,7 @@
         <v>0.009343206072515067</v>
       </c>
       <c r="G356">
-        <v>0.01855755299186846</v>
+        <v>0.01855755299186845</v>
       </c>
     </row>
     <row r="357" spans="1:7">
@@ -8606,7 +8606,7 @@
         <v>0.009343206072515067</v>
       </c>
       <c r="G357">
-        <v>0.01855755299186846</v>
+        <v>0.01855755299186845</v>
       </c>
     </row>
     <row r="358" spans="1:7">
@@ -8629,7 +8629,7 @@
         <v>0.009343206072515067</v>
       </c>
       <c r="G358">
-        <v>0.01855755299186846</v>
+        <v>0.01855755299186845</v>
       </c>
     </row>
     <row r="359" spans="1:7">
@@ -8637,7 +8637,7 @@
         <v>14.875</v>
       </c>
       <c r="B359">
-        <v>-565.6854249492366</v>
+        <v>-565.6854249492364</v>
       </c>
       <c r="C359">
         <v>-0.1</v>
@@ -8652,7 +8652,7 @@
         <v>0.009343206072515067</v>
       </c>
       <c r="G359">
-        <v>0.01855755299186846</v>
+        <v>0.01855755299186845</v>
       </c>
     </row>
     <row r="360" spans="1:7">
@@ -8675,7 +8675,7 @@
         <v>0.009343206072515067</v>
       </c>
       <c r="G360">
-        <v>0.01855755299186846</v>
+        <v>0.01855755299186845</v>
       </c>
     </row>
     <row r="361" spans="1:7">
@@ -8698,7 +8698,7 @@
         <v>0.009343206072515067</v>
       </c>
       <c r="G361">
-        <v>0.01855755299186846</v>
+        <v>0.01855755299186845</v>
       </c>
     </row>
     <row r="362" spans="1:7">
@@ -8721,7 +8721,7 @@
         <v>0.009343206072515067</v>
       </c>
       <c r="G362">
-        <v>0.01855755299186846</v>
+        <v>0.01855755299186845</v>
       </c>
     </row>
     <row r="363" spans="1:7">
@@ -8744,7 +8744,7 @@
         <v>0.009343206072515067</v>
       </c>
       <c r="G363">
-        <v>0.01855755299186846</v>
+        <v>0.01855755299186845</v>
       </c>
     </row>
     <row r="364" spans="1:7">
@@ -8767,7 +8767,7 @@
         <v>0.009343206072515067</v>
       </c>
       <c r="G364">
-        <v>0.01855755299186846</v>
+        <v>0.01855755299186845</v>
       </c>
     </row>
     <row r="365" spans="1:7">
@@ -8790,7 +8790,7 @@
         <v>0.009343206072515067</v>
       </c>
       <c r="G365">
-        <v>0.01855755299186846</v>
+        <v>0.01855755299186845</v>
       </c>
     </row>
     <row r="366" spans="1:7">
@@ -8813,7 +8813,7 @@
         <v>0.009343206072515067</v>
       </c>
       <c r="G366">
-        <v>0.01855755299186846</v>
+        <v>0.01855755299186845</v>
       </c>
     </row>
     <row r="367" spans="1:7">
@@ -8836,7 +8836,7 @@
         <v>0.009343206072515067</v>
       </c>
       <c r="G367">
-        <v>0.01855755299186846</v>
+        <v>0.01855755299186845</v>
       </c>
     </row>
     <row r="368" spans="1:7">
@@ -8847,7 +8847,7 @@
         <v>2.745189568127154E-12</v>
       </c>
       <c r="C368">
-        <v>8.374006566735033E-16</v>
+        <v>8.374006566735034E-16</v>
       </c>
       <c r="D368">
         <v>1.694116700343449</v>
@@ -8859,7 +8859,7 @@
         <v>0.009343206072515067</v>
       </c>
       <c r="G368">
-        <v>0.01855755299186846</v>
+        <v>0.01855755299186844</v>
       </c>
     </row>
     <row r="369" spans="1:7">
@@ -8882,7 +8882,7 @@
         <v>0.009341950184535468</v>
       </c>
       <c r="G369">
-        <v>0.01840182288239825</v>
+        <v>0.01840182288239824</v>
       </c>
     </row>
     <row r="370" spans="1:7">
@@ -8905,7 +8905,7 @@
         <v>0.009339553094076103</v>
       </c>
       <c r="G370">
-        <v>0.01810458366543693</v>
+        <v>0.01810458366543691</v>
       </c>
     </row>
     <row r="371" spans="1:7">
@@ -8913,7 +8913,7 @@
         <v>15.375</v>
       </c>
       <c r="B371">
-        <v>565.6854249492385</v>
+        <v>565.6854249492384</v>
       </c>
       <c r="C371">
         <v>0.1652369738538245</v>
@@ -8928,7 +8928,7 @@
         <v>0.009336242371985317</v>
       </c>
       <c r="G371">
-        <v>0.0176940541261795</v>
+        <v>0.01769405412617948</v>
       </c>
     </row>
     <row r="372" spans="1:7">
@@ -8951,7 +8951,7 @@
         <v>0.009332323609381656</v>
       </c>
       <c r="G372">
-        <v>0.01720812756332544</v>
+        <v>0.01720812756332543</v>
       </c>
     </row>
     <row r="373" spans="1:7">
@@ -8974,7 +8974,7 @@
         <v>0.00932813560521069</v>
       </c>
       <c r="G373">
-        <v>0.01668881504612555</v>
+        <v>0.01668881504612554</v>
       </c>
     </row>
     <row r="374" spans="1:7">
@@ -8997,7 +8997,7 @@
         <v>0.009324006123127684</v>
       </c>
       <c r="G374">
-        <v>0.01617675926783278</v>
+        <v>0.01617675926783276</v>
       </c>
     </row>
     <row r="375" spans="1:7">
@@ -9020,7 +9020,7 @@
         <v>0.009320217703700846</v>
       </c>
       <c r="G375">
-        <v>0.01570699525890494</v>
+        <v>0.01570699525890493</v>
       </c>
     </row>
     <row r="376" spans="1:7">
@@ -9043,7 +9043,7 @@
         <v>0.009316988954389245</v>
       </c>
       <c r="G376">
-        <v>0.01530663034426637</v>
+        <v>0.01530663034426636</v>
       </c>
     </row>
     <row r="377" spans="1:7">
@@ -9066,7 +9066,7 @@
         <v>0.009314471382824712</v>
       </c>
       <c r="G377">
-        <v>0.01499445147026426</v>
+        <v>0.01499445147026425</v>
       </c>
     </row>
     <row r="378" spans="1:7">
@@ -9089,7 +9089,7 @@
         <v>0.009312757483125947</v>
       </c>
       <c r="G378">
-        <v>0.01478192790761731</v>
+        <v>0.01478192790761729</v>
       </c>
     </row>
     <row r="379" spans="1:7">
@@ -9112,7 +9112,7 @@
         <v>0.009311893885198987</v>
       </c>
       <c r="G379">
-        <v>0.0146748417646742</v>
+        <v>0.01467484176467418</v>
       </c>
     </row>
     <row r="380" spans="1:7">
@@ -9135,7 +9135,7 @@
         <v>0.009311893885198987</v>
       </c>
       <c r="G380">
-        <v>0.01467484176467419</v>
+        <v>0.01467484176467418</v>
       </c>
     </row>
     <row r="381" spans="1:7">
@@ -9158,7 +9158,7 @@
         <v>0.009311893885198987</v>
       </c>
       <c r="G381">
-        <v>0.01467484176467419</v>
+        <v>0.01467484176467418</v>
       </c>
     </row>
     <row r="382" spans="1:7">
@@ -9181,7 +9181,7 @@
         <v>0.009311893885198987</v>
       </c>
       <c r="G382">
-        <v>0.01467484176467419</v>
+        <v>0.01467484176467418</v>
       </c>
     </row>
     <row r="383" spans="1:7">
@@ -9189,7 +9189,7 @@
         <v>15.875</v>
       </c>
       <c r="B383">
-        <v>-565.6854249492322</v>
+        <v>-565.6854249492324</v>
       </c>
       <c r="C383">
         <v>-0.1</v>
@@ -9204,7 +9204,7 @@
         <v>0.009311893885198987</v>
       </c>
       <c r="G383">
-        <v>0.01467484176467419</v>
+        <v>0.01467484176467418</v>
       </c>
     </row>
     <row r="384" spans="1:7">
@@ -9227,7 +9227,7 @@
         <v>0.009311893885198987</v>
       </c>
       <c r="G384">
-        <v>0.01467484176467419</v>
+        <v>0.01467484176467418</v>
       </c>
     </row>
     <row r="385" spans="1:7">
@@ -9250,7 +9250,7 @@
         <v>0.009311893885198987</v>
       </c>
       <c r="G385">
-        <v>0.01467484176467419</v>
+        <v>0.01467484176467418</v>
       </c>
     </row>
     <row r="386" spans="1:7">
@@ -9273,7 +9273,7 @@
         <v>0.009311893885198987</v>
       </c>
       <c r="G386">
-        <v>0.01467484176467419</v>
+        <v>0.01467484176467418</v>
       </c>
     </row>
     <row r="387" spans="1:7">
@@ -9296,7 +9296,7 @@
         <v>0.009311893885198987</v>
       </c>
       <c r="G387">
-        <v>0.01467484176467419</v>
+        <v>0.01467484176467418</v>
       </c>
     </row>
     <row r="388" spans="1:7">
@@ -9319,7 +9319,7 @@
         <v>0.009311893885198987</v>
       </c>
       <c r="G388">
-        <v>0.01467484176467419</v>
+        <v>0.01467484176467418</v>
       </c>
     </row>
     <row r="389" spans="1:7">
@@ -9342,7 +9342,7 @@
         <v>0.009311893885198987</v>
       </c>
       <c r="G389">
-        <v>0.01467484176467419</v>
+        <v>0.01467484176467418</v>
       </c>
     </row>
     <row r="390" spans="1:7">
@@ -9350,7 +9350,7 @@
         <v>16.16666666666666</v>
       </c>
       <c r="B390">
-        <v>-400.0000000000047</v>
+        <v>-400.0000000000048</v>
       </c>
       <c r="C390">
         <v>-0.1</v>
@@ -9365,7 +9365,7 @@
         <v>0.009311893885198987</v>
       </c>
       <c r="G390">
-        <v>0.01467484176467419</v>
+        <v>0.01467484176467418</v>
       </c>
     </row>
     <row r="391" spans="1:7">
@@ -9388,7 +9388,7 @@
         <v>0.009311893885198987</v>
       </c>
       <c r="G391">
-        <v>0.01467484176467419</v>
+        <v>0.01467484176467418</v>
       </c>
     </row>
     <row r="392" spans="1:7">
@@ -9411,7 +9411,7 @@
         <v>0.009311893885198987</v>
       </c>
       <c r="G392">
-        <v>0.01467484176467419</v>
+        <v>0.01467484176467418</v>
       </c>
     </row>
     <row r="393" spans="1:7">
@@ -9422,7 +9422,7 @@
         <v>207.0552360820202</v>
       </c>
       <c r="C393">
-        <v>0.05840394319178467</v>
+        <v>0.05840394319178468</v>
       </c>
       <c r="D393">
         <v>1.721229739326625</v>
@@ -9434,7 +9434,7 @@
         <v>0.009310716859770262</v>
       </c>
       <c r="G393">
-        <v>0.0145288906115123</v>
+        <v>0.01452889061151228</v>
       </c>
     </row>
     <row r="394" spans="1:7">
@@ -9457,7 +9457,7 @@
         <v>0.009308471187287863</v>
       </c>
       <c r="G394">
-        <v>0.01425042722369489</v>
+        <v>0.01425042722369487</v>
       </c>
     </row>
     <row r="395" spans="1:7">
@@ -9480,7 +9480,7 @@
         <v>0.009305371964958153</v>
       </c>
       <c r="G395">
-        <v>0.01386612365481093</v>
+        <v>0.01386612365481091</v>
       </c>
     </row>
     <row r="396" spans="1:7">
@@ -9503,7 +9503,7 @@
         <v>0.009301707436019546</v>
       </c>
       <c r="G396">
-        <v>0.01341172206642367</v>
+        <v>0.01341172206642366</v>
       </c>
     </row>
     <row r="397" spans="1:7">
@@ -9526,7 +9526,7 @@
         <v>0.009297796067362991</v>
       </c>
       <c r="G397">
-        <v>0.01292671235301077</v>
+        <v>0.01292671235301075</v>
       </c>
     </row>
     <row r="398" spans="1:7">
@@ -9549,7 +9549,7 @@
         <v>0.009293944560748096</v>
       </c>
       <c r="G398">
-        <v>0.01244912553276383</v>
+        <v>0.01244912553276382</v>
       </c>
     </row>
     <row r="399" spans="1:7">
@@ -9572,7 +9572,7 @@
         <v>0.009290415863534808</v>
       </c>
       <c r="G399">
-        <v>0.01201156707831616</v>
+        <v>0.01201156707831615</v>
       </c>
     </row>
     <row r="400" spans="1:7">
@@ -9595,7 +9595,7 @@
         <v>0.009287412136104171</v>
       </c>
       <c r="G400">
-        <v>0.01163910487691719</v>
+        <v>0.01163910487691718</v>
       </c>
     </row>
     <row r="401" spans="1:7">
@@ -9603,7 +9603,7 @@
         <v>16.625</v>
       </c>
       <c r="B401">
-        <v>565.6854249492367</v>
+        <v>565.6854249492368</v>
       </c>
       <c r="C401">
         <v>0.1105019934334896</v>
@@ -9618,7 +9618,7 @@
         <v>0.009285072448982704</v>
       </c>
       <c r="G401">
-        <v>0.01134898367385528</v>
+        <v>0.01134898367385527</v>
       </c>
     </row>
     <row r="402" spans="1:7">
@@ -9641,7 +9641,7 @@
         <v>0.009283480928724362</v>
       </c>
       <c r="G402">
-        <v>0.01115163516182096</v>
+        <v>0.01115163516182094</v>
       </c>
     </row>
     <row r="403" spans="1:7">
@@ -9652,7 +9652,7 @@
         <v>207.0552360820236</v>
       </c>
       <c r="C403">
-        <v>0.03756364232566331</v>
+        <v>0.03756364232566332</v>
       </c>
       <c r="D403">
         <v>1.820762610999134</v>
@@ -9664,7 +9664,7 @@
         <v>0.009282679431130116</v>
       </c>
       <c r="G403">
-        <v>0.01105224946013451</v>
+        <v>0.01105224946013449</v>
       </c>
     </row>
     <row r="404" spans="1:7">
@@ -9687,7 +9687,7 @@
         <v>0.009282679431130116</v>
       </c>
       <c r="G404">
-        <v>0.01105224946013451</v>
+        <v>0.01105224946013449</v>
       </c>
     </row>
     <row r="405" spans="1:7">
@@ -9710,7 +9710,7 @@
         <v>0.009282679431130116</v>
       </c>
       <c r="G405">
-        <v>0.01105224946013451</v>
+        <v>0.01105224946013449</v>
       </c>
     </row>
     <row r="406" spans="1:7">
@@ -9733,7 +9733,7 @@
         <v>0.009282679431130116</v>
       </c>
       <c r="G406">
-        <v>0.01105224946013451</v>
+        <v>0.01105224946013449</v>
       </c>
     </row>
     <row r="407" spans="1:7">
@@ -9756,7 +9756,7 @@
         <v>0.009282679431130116</v>
       </c>
       <c r="G407">
-        <v>0.01105224946013451</v>
+        <v>0.01105224946013449</v>
       </c>
     </row>
     <row r="408" spans="1:7">
@@ -9779,7 +9779,7 @@
         <v>0.009282679431130116</v>
       </c>
       <c r="G408">
-        <v>0.01105224946013451</v>
+        <v>0.01105224946013449</v>
       </c>
     </row>
     <row r="409" spans="1:7">
@@ -9802,7 +9802,7 @@
         <v>0.009282679431130116</v>
       </c>
       <c r="G409">
-        <v>0.01105224946013451</v>
+        <v>0.01105224946013449</v>
       </c>
     </row>
     <row r="410" spans="1:7">
@@ -9825,7 +9825,7 @@
         <v>0.009282679431130116</v>
       </c>
       <c r="G410">
-        <v>0.01105224946013451</v>
+        <v>0.01105224946013449</v>
       </c>
     </row>
     <row r="411" spans="1:7">
@@ -9848,7 +9848,7 @@
         <v>0.009282679431130116</v>
       </c>
       <c r="G411">
-        <v>0.01105224946013451</v>
+        <v>0.01105224946013449</v>
       </c>
     </row>
     <row r="412" spans="1:7">
@@ -9871,7 +9871,7 @@
         <v>0.009282679431130116</v>
       </c>
       <c r="G412">
-        <v>0.01105224946013451</v>
+        <v>0.01105224946013449</v>
       </c>
     </row>
     <row r="413" spans="1:7">
@@ -9894,7 +9894,7 @@
         <v>0.009282679431130116</v>
       </c>
       <c r="G413">
-        <v>0.01105224946013451</v>
+        <v>0.01105224946013449</v>
       </c>
     </row>
     <row r="414" spans="1:7">
@@ -9917,7 +9917,7 @@
         <v>0.009282679431130116</v>
       </c>
       <c r="G414">
-        <v>0.01105224946013451</v>
+        <v>0.01105224946013449</v>
       </c>
     </row>
     <row r="415" spans="1:7">
@@ -9940,7 +9940,7 @@
         <v>0.009282679431130116</v>
       </c>
       <c r="G415">
-        <v>0.01105224946013451</v>
+        <v>0.01105224946013449</v>
       </c>
     </row>
     <row r="416" spans="1:7">
@@ -9963,7 +9963,7 @@
         <v>0.009282679431130116</v>
       </c>
       <c r="G416">
-        <v>0.01105224946013451</v>
+        <v>0.01105224946013449</v>
       </c>
     </row>
     <row r="417" spans="1:7">
@@ -9986,7 +9986,7 @@
         <v>0.009281554744169803</v>
       </c>
       <c r="G417">
-        <v>0.01091278827705568</v>
+        <v>0.01091278827705566</v>
       </c>
     </row>
     <row r="418" spans="1:7">
@@ -10009,7 +10009,7 @@
         <v>0.009279409486231537</v>
       </c>
       <c r="G418">
-        <v>0.01064677629271067</v>
+        <v>0.01064677629271065</v>
       </c>
     </row>
     <row r="419" spans="1:7">
@@ -10032,7 +10032,7 @@
         <v>0.009276450319776213</v>
       </c>
       <c r="G419">
-        <v>0.01027983965225057</v>
+        <v>0.01027983965225055</v>
       </c>
     </row>
     <row r="420" spans="1:7">
@@ -10055,7 +10055,7 @@
         <v>0.009272953813650503</v>
       </c>
       <c r="G420">
-        <v>0.009846272892662532</v>
+        <v>0.009846272892662518</v>
       </c>
     </row>
     <row r="421" spans="1:7">
@@ -10078,7 +10078,7 @@
         <v>0.009269224854348423</v>
       </c>
       <c r="G421">
-        <v>0.009383881939204511</v>
+        <v>0.009383881939204497</v>
       </c>
     </row>
     <row r="422" spans="1:7">
@@ -10089,7 +10089,7 @@
         <v>800</v>
       </c>
       <c r="C422">
-        <v>0.1756455134722506</v>
+        <v>0.1756455134722507</v>
       </c>
       <c r="D422">
         <v>1.792569530355765</v>
@@ -10101,7 +10101,7 @@
         <v>0.009265556201321247</v>
       </c>
       <c r="G422">
-        <v>0.008928968963834782</v>
+        <v>0.008928968963834768</v>
       </c>
     </row>
     <row r="423" spans="1:7">
@@ -10124,7 +10124,7 @@
         <v>0.009262197956288909</v>
       </c>
       <c r="G423">
-        <v>0.008512546579824899</v>
+        <v>0.008512546579824885</v>
       </c>
     </row>
     <row r="424" spans="1:7">
@@ -10147,7 +10147,7 @@
         <v>0.009259341602615715</v>
       </c>
       <c r="G424">
-        <v>0.008158358724348834</v>
+        <v>0.00815835872434882</v>
       </c>
     </row>
     <row r="425" spans="1:7">
@@ -10170,7 +10170,7 @@
         <v>0.009257118217328162</v>
       </c>
       <c r="G425">
-        <v>0.007882658948692259</v>
+        <v>0.007882658948692245</v>
       </c>
     </row>
     <row r="426" spans="1:7">
@@ -10193,7 +10193,7 @@
         <v>0.009255606604620308</v>
       </c>
       <c r="G426">
-        <v>0.007695218972918313</v>
+        <v>0.007695218972918299</v>
       </c>
     </row>
     <row r="427" spans="1:7">
@@ -10216,7 +10216,7 @@
         <v>0.009254845619910081</v>
       </c>
       <c r="G427">
-        <v>0.007600856868850162</v>
+        <v>0.007600856868850149</v>
       </c>
     </row>
     <row r="428" spans="1:7">
@@ -10239,7 +10239,7 @@
         <v>0.009254845619910081</v>
       </c>
       <c r="G428">
-        <v>0.007600856868850162</v>
+        <v>0.007600856868850149</v>
       </c>
     </row>
     <row r="429" spans="1:7">
@@ -10262,7 +10262,7 @@
         <v>0.009254845619910081</v>
       </c>
       <c r="G429">
-        <v>0.007600856868850162</v>
+        <v>0.007600856868850149</v>
       </c>
     </row>
     <row r="430" spans="1:7">
@@ -10285,7 +10285,7 @@
         <v>0.009254845619910081</v>
       </c>
       <c r="G430">
-        <v>0.007600856868850162</v>
+        <v>0.007600856868850149</v>
       </c>
     </row>
     <row r="431" spans="1:7">
@@ -10293,7 +10293,7 @@
         <v>17.875</v>
       </c>
       <c r="B431">
-        <v>-565.6854249492321</v>
+        <v>-565.685424949232</v>
       </c>
       <c r="C431">
         <v>-0.1</v>
@@ -10308,7 +10308,7 @@
         <v>0.009254845619910081</v>
       </c>
       <c r="G431">
-        <v>0.007600856868850162</v>
+        <v>0.007600856868850149</v>
       </c>
     </row>
     <row r="432" spans="1:7">
@@ -10331,7 +10331,7 @@
         <v>0.009254845619910081</v>
       </c>
       <c r="G432">
-        <v>0.007600856868850162</v>
+        <v>0.007600856868850149</v>
       </c>
     </row>
     <row r="433" spans="1:7">
@@ -10354,7 +10354,7 @@
         <v>0.009254845619910081</v>
       </c>
       <c r="G433">
-        <v>0.007600856868850162</v>
+        <v>0.007600856868850149</v>
       </c>
     </row>
     <row r="434" spans="1:7">
@@ -10377,7 +10377,7 @@
         <v>0.009254845619910081</v>
       </c>
       <c r="G434">
-        <v>0.007600856868850162</v>
+        <v>0.007600856868850149</v>
       </c>
     </row>
     <row r="435" spans="1:7">
@@ -10385,7 +10385,7 @@
         <v>18.04166666666666</v>
       </c>
       <c r="B435">
-        <v>-772.7406610312527</v>
+        <v>-772.7406610312526</v>
       </c>
       <c r="C435">
         <v>-0.1</v>
@@ -10400,7 +10400,7 @@
         <v>0.009254845619910081</v>
       </c>
       <c r="G435">
-        <v>0.007600856868850162</v>
+        <v>0.007600856868850149</v>
       </c>
     </row>
     <row r="436" spans="1:7">
@@ -10423,7 +10423,7 @@
         <v>0.009254845619910081</v>
       </c>
       <c r="G436">
-        <v>0.007600856868850162</v>
+        <v>0.007600856868850149</v>
       </c>
     </row>
     <row r="437" spans="1:7">
@@ -10431,7 +10431,7 @@
         <v>18.125</v>
       </c>
       <c r="B437">
-        <v>-565.6854249492391</v>
+        <v>-565.6854249492389</v>
       </c>
       <c r="C437">
         <v>-0.1</v>
@@ -10446,7 +10446,7 @@
         <v>0.009254845619910081</v>
       </c>
       <c r="G437">
-        <v>0.007600856868850162</v>
+        <v>0.007600856868850149</v>
       </c>
     </row>
     <row r="438" spans="1:7">
@@ -10469,7 +10469,7 @@
         <v>0.009254845619910081</v>
       </c>
       <c r="G438">
-        <v>0.007600856868850162</v>
+        <v>0.007600856868850149</v>
       </c>
     </row>
     <row r="439" spans="1:7">
@@ -10492,7 +10492,7 @@
         <v>0.009254845619910081</v>
       </c>
       <c r="G439">
-        <v>0.007600856868850162</v>
+        <v>0.007600856868850149</v>
       </c>
     </row>
     <row r="440" spans="1:7">
@@ -10515,7 +10515,7 @@
         <v>0.009254845619910081</v>
       </c>
       <c r="G440">
-        <v>0.007600856868850162</v>
+        <v>0.007600856868850149</v>
       </c>
     </row>
     <row r="441" spans="1:7">
@@ -10538,7 +10538,7 @@
         <v>0.009253729514918702</v>
       </c>
       <c r="G441">
-        <v>0.007462459849919095</v>
+        <v>0.007462459849919082</v>
       </c>
     </row>
     <row r="442" spans="1:7">
@@ -10561,7 +10561,7 @@
         <v>0.009251600743492534</v>
       </c>
       <c r="G442">
-        <v>0.007198492193074215</v>
+        <v>0.007198492193074202</v>
       </c>
     </row>
     <row r="443" spans="1:7">
@@ -10584,7 +10584,7 @@
         <v>0.009248664635096939</v>
       </c>
       <c r="G443">
-        <v>0.00683441475202054</v>
+        <v>0.006834414752020526</v>
       </c>
     </row>
     <row r="444" spans="1:7">
@@ -10607,7 +10607,7 @@
         <v>0.009245195912489563</v>
       </c>
       <c r="G444">
-        <v>0.006404293148705948</v>
+        <v>0.006404293148705934</v>
       </c>
     </row>
     <row r="445" spans="1:7">
@@ -10630,7 +10630,7 @@
         <v>0.009241497303036056</v>
       </c>
       <c r="G445">
-        <v>0.005945665576471094</v>
+        <v>0.00594566557647108</v>
       </c>
     </row>
     <row r="446" spans="1:7">
@@ -10653,7 +10653,7 @@
         <v>0.009237859321510868</v>
       </c>
       <c r="G446">
-        <v>0.005494555867347687</v>
+        <v>0.005494555867347673</v>
       </c>
     </row>
     <row r="447" spans="1:7">
@@ -10676,7 +10676,7 @@
         <v>0.009234529951634903</v>
       </c>
       <c r="G447">
-        <v>0.005081714002728028</v>
+        <v>0.005081714002728014</v>
       </c>
     </row>
     <row r="448" spans="1:7">
@@ -10699,7 +10699,7 @@
         <v>0.009231698843164316</v>
       </c>
       <c r="G448">
-        <v>0.004730656552375177</v>
+        <v>0.004730656552375163</v>
       </c>
     </row>
     <row r="449" spans="1:7">
@@ -10710,7 +10710,7 @@
         <v>565.6854249492451</v>
       </c>
       <c r="C449">
-        <v>0.1033648434741211</v>
+        <v>0.1033648434741212</v>
       </c>
       <c r="D449">
         <v>1.823869003743227</v>
@@ -10722,7 +10722,7 @@
         <v>0.009229495609968821</v>
       </c>
       <c r="G449">
-        <v>0.004457455636133849</v>
+        <v>0.004457455636133835</v>
       </c>
     </row>
     <row r="450" spans="1:7">
@@ -10733,7 +10733,7 @@
         <v>400.0000000000027</v>
       </c>
       <c r="C450">
-        <v>0.06995969912317666</v>
+        <v>0.06995969912317665</v>
       </c>
       <c r="D450">
         <v>1.829185559024142</v>
@@ -10745,7 +10745,7 @@
         <v>0.009227997988762929</v>
       </c>
       <c r="G450">
-        <v>0.004271750606603291</v>
+        <v>0.004271750606603277</v>
       </c>
     </row>
     <row r="451" spans="1:7">
@@ -10768,7 +10768,7 @@
         <v>0.009227244154770026</v>
       </c>
       <c r="G451">
-        <v>0.0041782751914832</v>
+        <v>0.004178275191483186</v>
       </c>
     </row>
     <row r="452" spans="1:7">
@@ -10791,7 +10791,7 @@
         <v>0.009227244154770026</v>
       </c>
       <c r="G452">
-        <v>0.0041782751914832</v>
+        <v>0.004178275191483186</v>
       </c>
     </row>
     <row r="453" spans="1:7">
@@ -10814,7 +10814,7 @@
         <v>0.009227244154770026</v>
       </c>
       <c r="G453">
-        <v>0.0041782751914832</v>
+        <v>0.004178275191483186</v>
       </c>
     </row>
     <row r="454" spans="1:7">
@@ -10837,7 +10837,7 @@
         <v>0.009227244154770026</v>
       </c>
       <c r="G454">
-        <v>0.0041782751914832</v>
+        <v>0.004178275191483186</v>
       </c>
     </row>
     <row r="455" spans="1:7">
@@ -10860,7 +10860,7 @@
         <v>0.009227244154770026</v>
       </c>
       <c r="G455">
-        <v>0.0041782751914832</v>
+        <v>0.004178275191483186</v>
       </c>
     </row>
     <row r="456" spans="1:7">
@@ -10883,7 +10883,7 @@
         <v>0.009227244154770026</v>
       </c>
       <c r="G456">
-        <v>0.0041782751914832</v>
+        <v>0.004178275191483186</v>
       </c>
     </row>
     <row r="457" spans="1:7">
@@ -10906,7 +10906,7 @@
         <v>0.009227244154770026</v>
       </c>
       <c r="G457">
-        <v>0.0041782751914832</v>
+        <v>0.004178275191483186</v>
       </c>
     </row>
     <row r="458" spans="1:7">
@@ -10929,7 +10929,7 @@
         <v>0.009227244154770026</v>
       </c>
       <c r="G458">
-        <v>0.0041782751914832</v>
+        <v>0.004178275191483186</v>
       </c>
     </row>
     <row r="459" spans="1:7">
@@ -10952,7 +10952,7 @@
         <v>0.009227244154770026</v>
       </c>
       <c r="G459">
-        <v>0.0041782751914832</v>
+        <v>0.004178275191483186</v>
       </c>
     </row>
     <row r="460" spans="1:7">
@@ -10975,7 +10975,7 @@
         <v>0.009227244154770026</v>
       </c>
       <c r="G460">
-        <v>0.0041782751914832</v>
+        <v>0.004178275191483186</v>
       </c>
     </row>
     <row r="461" spans="1:7">
@@ -10998,7 +10998,7 @@
         <v>0.009227244154770026</v>
       </c>
       <c r="G461">
-        <v>0.0041782751914832</v>
+        <v>0.004178275191483186</v>
       </c>
     </row>
     <row r="462" spans="1:7">
@@ -11021,7 +11021,7 @@
         <v>0.009227244154770026</v>
       </c>
       <c r="G462">
-        <v>0.0041782751914832</v>
+        <v>0.004178275191483186</v>
       </c>
     </row>
     <row r="463" spans="1:7">
@@ -11044,7 +11044,7 @@
         <v>0.009227244154770026</v>
       </c>
       <c r="G463">
-        <v>0.0041782751914832</v>
+        <v>0.004178275191483186</v>
       </c>
     </row>
     <row r="464" spans="1:7">
@@ -11067,7 +11067,7 @@
         <v>0.009227244154770026</v>
       </c>
       <c r="G464">
-        <v>0.0041782751914832</v>
+        <v>0.004178275191483186</v>
       </c>
     </row>
     <row r="465" spans="1:7">
@@ -11090,7 +11090,7 @@
         <v>0.009226161179495174</v>
       </c>
       <c r="G465">
-        <v>0.004043986257401488</v>
+        <v>0.004043986257401474</v>
       </c>
     </row>
     <row r="466" spans="1:7">
@@ -11113,7 +11113,7 @@
         <v>0.009224096109555891</v>
       </c>
       <c r="G466">
-        <v>0.003787917584930524</v>
+        <v>0.00378791758493051</v>
       </c>
     </row>
     <row r="467" spans="1:7">
@@ -11136,7 +11136,7 @@
         <v>0.009221249287794367</v>
       </c>
       <c r="G467">
-        <v>0.00343491168650146</v>
+        <v>0.003434911686501446</v>
       </c>
     </row>
     <row r="468" spans="1:7">
@@ -11159,7 +11159,7 @@
         <v>0.009217888608850755</v>
       </c>
       <c r="G468">
-        <v>0.003018187497493554</v>
+        <v>0.003018187497493541</v>
       </c>
     </row>
     <row r="469" spans="1:7">
@@ -11182,7 +11182,7 @@
         <v>0.00921430893975928</v>
       </c>
       <c r="G469">
-        <v>0.002574308530150721</v>
+        <v>0.002574308530150708</v>
       </c>
     </row>
     <row r="470" spans="1:7">
@@ -11205,7 +11205,7 @@
         <v>0.009210792777054166</v>
       </c>
       <c r="G470">
-        <v>0.002138304354716704</v>
+        <v>0.00213830435471669</v>
       </c>
     </row>
     <row r="471" spans="1:7">
@@ -11228,7 +11228,7 @@
         <v>0.009207580635161141</v>
       </c>
       <c r="G471">
-        <v>0.001739998759981437</v>
+        <v>0.001739998759981423</v>
       </c>
     </row>
     <row r="472" spans="1:7">
@@ -11251,7 +11251,7 @@
         <v>0.009204855536004253</v>
       </c>
       <c r="G472">
-        <v>0.001402086464527328</v>
+        <v>0.001402086464527314</v>
       </c>
     </row>
     <row r="473" spans="1:7">
@@ -11262,7 +11262,7 @@
         <v>565.6854249492412</v>
       </c>
       <c r="C473">
-        <v>0.09888758365712441</v>
+        <v>0.0988875836571244</v>
       </c>
       <c r="D473">
         <v>1.829324776703773</v>
@@ -11274,7 +11274,7 @@
         <v>0.009202741038228447</v>
       </c>
       <c r="G473">
-        <v>0.001139888740327462</v>
+        <v>0.001139888740327448</v>
       </c>
     </row>
     <row r="474" spans="1:7">
@@ -11297,7 +11297,7 @@
         <v>0.009201308722587963</v>
       </c>
       <c r="G474">
-        <v>0.0009622816009075976</v>
+        <v>0.0009622816009075839</v>
       </c>
     </row>
     <row r="475" spans="1:7">
@@ -11320,7 +11320,7 @@
         <v>0.009200590236457841</v>
       </c>
       <c r="G475">
-        <v>0.0008731893207724766</v>
+        <v>0.000873189320772463</v>
       </c>
     </row>
     <row r="476" spans="1:7">
@@ -11331,7 +11331,7 @@
         <v>6.663068956380142E-12</v>
       </c>
       <c r="C476">
-        <v>1.054599427850656E-15</v>
+        <v>1.054599427850655E-15</v>
       </c>
       <c r="D476">
         <v>1.83696012298942</v>
@@ -11343,7 +11343,7 @@
         <v>0.009200590236457841</v>
       </c>
       <c r="G476">
-        <v>0.0008731893207724738</v>
+        <v>0.0008731893207724602</v>
       </c>
     </row>
     <row r="477" spans="1:7">
@@ -11366,7 +11366,7 @@
         <v>0.009200590236457841</v>
       </c>
       <c r="G477">
-        <v>0.0008731893207724738</v>
+        <v>0.0008731893207724602</v>
       </c>
     </row>
     <row r="478" spans="1:7">
@@ -11389,7 +11389,7 @@
         <v>0.009200590236457841</v>
       </c>
       <c r="G478">
-        <v>0.0008731893207724738</v>
+        <v>0.0008731893207724602</v>
       </c>
     </row>
     <row r="479" spans="1:7">
@@ -11412,7 +11412,7 @@
         <v>0.009200590236457841</v>
       </c>
       <c r="G479">
-        <v>0.0008731893207724738</v>
+        <v>0.0008731893207724602</v>
       </c>
     </row>
     <row r="480" spans="1:7">
@@ -11435,7 +11435,7 @@
         <v>0.009200590236457841</v>
       </c>
       <c r="G480">
-        <v>0.0008731893207724738</v>
+        <v>0.0008731893207724602</v>
       </c>
     </row>
     <row r="481" spans="1:7">
@@ -11458,7 +11458,7 @@
         <v>0.009200590236457841</v>
       </c>
       <c r="G481">
-        <v>0.0008731893207724738</v>
+        <v>0.0008731893207724602</v>
       </c>
     </row>
     <row r="482" spans="1:7">
@@ -11481,7 +11481,7 @@
         <v>0.009200590236457841</v>
       </c>
       <c r="G482">
-        <v>0.0008731893207724738</v>
+        <v>0.0008731893207724602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>